<commit_message>
fix: fix flash map file.
</commit_message>
<xml_diff>
--- a/doc/SIGMeshFlashmap_20230328.xlsx
+++ b/doc/SIGMeshFlashmap_20230328.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540"/>
+    <workbookView windowWidth="17568" windowHeight="9420" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SIGMeshB85m512K" sheetId="12" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="190">
   <si>
     <t>SIG Mesh B85m 512K flash map</t>
   </si>
@@ -248,17 +248,152 @@
     <t>Sig Mesh Parameters 2(B91_mesh)</t>
   </si>
   <si>
+    <t>E0000</t>
+  </si>
+  <si>
     <t>F0000</t>
   </si>
   <si>
+    <t>E0FFF</t>
+  </si>
+  <si>
+    <t>5FFFF</t>
+  </si>
+  <si>
+    <t>E1000</t>
+  </si>
+  <si>
+    <t>60000</t>
+  </si>
+  <si>
     <t>reserved for future use</t>
+  </si>
+  <si>
+    <t>should not be used to store parameters unless without flash protection funtion</t>
+  </si>
+  <si>
+    <t>E1FFF</t>
+  </si>
+  <si>
+    <t>E2000</t>
+  </si>
+  <si>
+    <t>7FFFF</t>
+  </si>
+  <si>
+    <t>E2FFF</t>
+  </si>
+  <si>
+    <t>80000</t>
+  </si>
+  <si>
+    <t>E3000</t>
+  </si>
+  <si>
+    <t>E3FFF</t>
+  </si>
+  <si>
+    <t>DFFFF</t>
+  </si>
+  <si>
+    <t>E4000</t>
+  </si>
+  <si>
+    <t>E4FFF</t>
+  </si>
+  <si>
+    <t>E5000</t>
+  </si>
+  <si>
+    <t>EFFFF</t>
+  </si>
+  <si>
+    <t>E5FFF</t>
+  </si>
+  <si>
+    <t>E6000</t>
+  </si>
+  <si>
+    <t>E6FFF</t>
+  </si>
+  <si>
+    <t>F5FFF</t>
+  </si>
+  <si>
+    <t>E7000</t>
+  </si>
+  <si>
+    <t>F6000</t>
+  </si>
+  <si>
+    <t>E7FFF</t>
+  </si>
+  <si>
+    <t>E8000</t>
+  </si>
+  <si>
+    <t>FDFFF</t>
+  </si>
+  <si>
+    <t>E8FFF</t>
+  </si>
+  <si>
+    <t>FE000</t>
   </si>
   <si>
     <t>Frequency Offset (0xfe000)
 FLASH_ADR_STATIC_OOB(0xfe800)</t>
   </si>
   <si>
+    <t>E9000</t>
+  </si>
+  <si>
+    <t>E9FFF</t>
+  </si>
+  <si>
+    <t>FEFFF</t>
+  </si>
+  <si>
+    <t>EA000</t>
+  </si>
+  <si>
+    <t>FF000</t>
+  </si>
+  <si>
     <t>Mac (0xff000-0xff005)</t>
+  </si>
+  <si>
+    <t>EAFFF</t>
+  </si>
+  <si>
+    <t>EB000</t>
+  </si>
+  <si>
+    <t>FFFFF</t>
+  </si>
+  <si>
+    <t>EBFFF</t>
+  </si>
+  <si>
+    <t>EC000</t>
+  </si>
+  <si>
+    <t>ECFFF</t>
+  </si>
+  <si>
+    <t>ED000</t>
+  </si>
+  <si>
+    <t>EDFFF</t>
+  </si>
+  <si>
+    <t>EE000</t>
+  </si>
+  <si>
+    <t>EEFFF</t>
+  </si>
+  <si>
+    <t>EF000</t>
   </si>
   <si>
     <t>FLASH_ADR_MD_PROPERTY/FLASH_ADR_MD_DF_SBR/FLASH_ADR_MD_SOLI_PDU_RPL</t>
@@ -2191,24 +2326,24 @@
   <sheetPr/>
   <dimension ref="B1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+    <sheetView zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
       <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="9.25" style="6" customWidth="1"/>
-    <col min="3" max="3" width="30.625" customWidth="1"/>
+    <col min="3" max="3" width="30.6296296296296" customWidth="1"/>
     <col min="4" max="4" width="9.75" customWidth="1"/>
-    <col min="5" max="5" width="32.425" customWidth="1"/>
-    <col min="6" max="6" width="5.625" customWidth="1"/>
+    <col min="5" max="5" width="32.4259259259259" customWidth="1"/>
+    <col min="6" max="6" width="5.62962962962963" customWidth="1"/>
     <col min="7" max="7" width="5" customWidth="1"/>
-    <col min="8" max="8" width="9.875" style="6" customWidth="1"/>
-    <col min="9" max="9" width="35.1333333333333" customWidth="1"/>
-    <col min="10" max="10" width="10.375" customWidth="1"/>
-    <col min="12" max="12" width="9.11666666666667" customWidth="1"/>
-    <col min="13" max="13" width="31.125" customWidth="1"/>
+    <col min="8" max="8" width="9.87962962962963" style="6" customWidth="1"/>
+    <col min="9" max="9" width="35.1296296296296" customWidth="1"/>
+    <col min="10" max="10" width="10.3796296296296" customWidth="1"/>
+    <col min="12" max="12" width="9.12037037037037" customWidth="1"/>
+    <col min="13" max="13" width="31.1296296296296" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="39" customHeight="1" spans="2:14">
@@ -2261,7 +2396,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" ht="15.75" spans="2:14">
+    <row r="3" ht="15.6" spans="2:14">
       <c r="B3" s="184" t="s">
         <v>7</v>
       </c>
@@ -2293,7 +2428,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" ht="15.75" spans="2:14">
+    <row r="4" ht="15.6" spans="2:14">
       <c r="B4" s="13" t="s">
         <v>11</v>
       </c>
@@ -2313,7 +2448,7 @@
       <c r="M4" s="133"/>
       <c r="N4" s="52"/>
     </row>
-    <row r="5" ht="15.75" spans="2:14">
+    <row r="5" ht="15.6" spans="2:14">
       <c r="B5" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(B3)+D3*1024-1)</f>
         <v>2FFFF</v>
@@ -2342,7 +2477,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" ht="15.75" spans="2:14">
+    <row r="6" ht="15.6" spans="2:14">
       <c r="B6" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(B5)+1)</f>
         <v>30000</v>
@@ -2369,7 +2504,7 @@
       <c r="M6" s="137"/>
       <c r="N6" s="52"/>
     </row>
-    <row r="7" ht="15.75" spans="2:14">
+    <row r="7" ht="15.6" spans="2:14">
       <c r="B7" s="13" t="s">
         <v>11</v>
       </c>
@@ -2397,7 +2532,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" ht="15.75" spans="2:14">
+    <row r="8" ht="15.6" spans="2:14">
       <c r="B8" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(B6)+D6*1024-1)</f>
         <v>3FFFF</v>
@@ -2418,7 +2553,7 @@
       <c r="M8" s="145"/>
       <c r="N8" s="52"/>
     </row>
-    <row r="9" ht="15.75" spans="2:14">
+    <row r="9" ht="15.6" spans="2:14">
       <c r="B9" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(B8)+1)</f>
         <v>40000</v>
@@ -2451,7 +2586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" ht="15.75" spans="2:14">
+    <row r="10" ht="15.6" spans="2:14">
       <c r="B10" s="13" t="s">
         <v>11</v>
       </c>
@@ -2471,7 +2606,7 @@
       <c r="M10" s="151"/>
       <c r="N10" s="52"/>
     </row>
-    <row r="11" ht="15.75" spans="2:14">
+    <row r="11" ht="15.6" spans="2:14">
       <c r="B11" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(B9)+D9*1024-1)</f>
         <v>6FFFF</v>
@@ -2500,7 +2635,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" ht="15.75" spans="2:14">
+    <row r="12" ht="15.6" spans="2:14">
       <c r="B12" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(B11)+1)</f>
         <v>70000</v>
@@ -2527,7 +2662,7 @@
       <c r="M12" s="151"/>
       <c r="N12" s="52"/>
     </row>
-    <row r="13" ht="15.75" spans="2:14">
+    <row r="13" ht="15.6" spans="2:14">
       <c r="B13" s="13" t="s">
         <v>11</v>
       </c>
@@ -2555,7 +2690,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" ht="15.75" spans="2:14">
+    <row r="14" ht="15.6" spans="2:14">
       <c r="B14" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(B12)+D12*1024-1)</f>
         <v>75FFF</v>
@@ -2599,7 +2734,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" ht="15.75" spans="2:10">
+    <row r="16" ht="15.6" spans="2:10">
       <c r="B16" s="13" t="s">
         <v>11</v>
       </c>
@@ -2613,7 +2748,7 @@
       <c r="I16" s="88"/>
       <c r="J16" s="52"/>
     </row>
-    <row r="17" ht="15.75" spans="2:14">
+    <row r="17" ht="15.6" spans="2:14">
       <c r="B17" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(B15)+D15*1024-1)</f>
         <v>76FFF</v>
@@ -2638,7 +2773,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" ht="15.75" spans="2:14">
+    <row r="18" ht="15.6" spans="2:14">
       <c r="B18" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(B17)+1)</f>
         <v>77000</v>
@@ -2665,7 +2800,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" ht="15.75" spans="2:14">
+    <row r="19" ht="15.6" spans="2:14">
       <c r="B19" s="13" t="s">
         <v>11</v>
       </c>
@@ -2689,7 +2824,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" ht="15.75" spans="2:14">
+    <row r="20" ht="15.6" spans="2:14">
       <c r="B20" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(B18)+D18*1024-1)</f>
         <v>77FFF</v>
@@ -2710,7 +2845,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" ht="15.75" spans="2:14">
+    <row r="21" ht="15.6" spans="2:14">
       <c r="B21" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(B20)+1)</f>
         <v>78000</v>
@@ -2741,7 +2876,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" ht="15.75" spans="2:14">
+    <row r="22" ht="15.6" spans="2:14">
       <c r="B22" s="13" t="s">
         <v>11</v>
       </c>
@@ -2761,7 +2896,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" ht="15.75" spans="2:14">
+    <row r="23" ht="15.6" spans="2:14">
       <c r="B23" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(B21)+D21*1024-1)</f>
         <v>7FFFF</v>
@@ -2786,7 +2921,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" ht="15.75" spans="8:14">
+    <row r="24" ht="15.6" spans="8:14">
       <c r="H24" s="14" t="str">
         <f t="shared" si="6"/>
         <v>3AFFF</v>
@@ -2800,7 +2935,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" ht="15.75" spans="8:14">
+    <row r="25" ht="15.6" spans="8:14">
       <c r="H25" s="9" t="str">
         <f t="shared" si="7"/>
         <v>3B000</v>
@@ -2818,7 +2953,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" ht="15.75" spans="8:14">
+    <row r="26" ht="15.6" spans="8:14">
       <c r="H26" s="14" t="str">
         <f t="shared" si="6"/>
         <v>3BFFF</v>
@@ -2850,7 +2985,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" ht="15.75" spans="8:14">
+    <row r="28" ht="15.6" spans="8:14">
       <c r="H28" s="14" t="str">
         <f t="shared" ref="H28:H32" si="8">DEC2HEX(HEX2DEC(H27)+J27*1024-1)</f>
         <v>3CFFF</v>
@@ -2864,7 +2999,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" ht="15.75" spans="8:14">
+    <row r="29" ht="15.6" spans="8:14">
       <c r="H29" s="9" t="str">
         <f t="shared" ref="H29:H33" si="9">DEC2HEX(HEX2DEC(H28)+1)</f>
         <v>3D000</v>
@@ -2928,7 +3063,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" ht="15.75" spans="8:14">
+    <row r="33" ht="15.6" spans="8:14">
       <c r="H33" s="9" t="str">
         <f t="shared" si="9"/>
         <v>3F000</v>
@@ -2946,7 +3081,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" ht="15.75" spans="8:14">
+    <row r="34" ht="15.6" spans="8:14">
       <c r="H34" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(H33)+J33*1024-1)</f>
         <v>3FFFF</v>
@@ -3091,19 +3226,19 @@
       <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="9.25" style="6" customWidth="1"/>
-    <col min="3" max="3" width="30.625" customWidth="1"/>
+    <col min="3" max="3" width="30.6296296296296" customWidth="1"/>
     <col min="4" max="4" width="9.75" customWidth="1"/>
-    <col min="5" max="5" width="32.425" customWidth="1"/>
-    <col min="6" max="6" width="5.625" customWidth="1"/>
-    <col min="7" max="7" width="4.375" customWidth="1"/>
+    <col min="5" max="5" width="32.4259259259259" customWidth="1"/>
+    <col min="6" max="6" width="5.62962962962963" customWidth="1"/>
+    <col min="7" max="7" width="4.37962962962963" customWidth="1"/>
     <col min="8" max="8" width="5" customWidth="1"/>
-    <col min="9" max="9" width="9.875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="35.1333333333333" customWidth="1"/>
-    <col min="11" max="11" width="10.375" customWidth="1"/>
+    <col min="9" max="9" width="9.87962962962963" style="6" customWidth="1"/>
+    <col min="10" max="10" width="35.1296296296296" customWidth="1"/>
+    <col min="11" max="11" width="10.3796296296296" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="39" customHeight="1" spans="2:11">
@@ -3142,7 +3277,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" ht="15.75" spans="2:11">
+    <row r="3" ht="15.6" spans="2:11">
       <c r="B3" s="184" t="s">
         <v>7</v>
       </c>
@@ -3164,7 +3299,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" ht="15.75" spans="2:11">
+    <row r="4" ht="15.6" spans="2:11">
       <c r="B4" s="13" t="s">
         <v>11</v>
       </c>
@@ -3178,7 +3313,7 @@
       <c r="J4" s="50"/>
       <c r="K4" s="52"/>
     </row>
-    <row r="5" ht="15.75" spans="2:11">
+    <row r="5" ht="15.6" spans="2:11">
       <c r="B5" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(B3)+D3*1024-1)</f>
         <v>3EFFF</v>
@@ -3197,7 +3332,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" ht="15.75" spans="2:11">
+    <row r="6" ht="15.6" spans="2:11">
       <c r="B6" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(B5)+1)</f>
         <v>3F000</v>
@@ -3218,7 +3353,7 @@
       <c r="J6" s="55"/>
       <c r="K6" s="52"/>
     </row>
-    <row r="7" ht="15.75" spans="2:11">
+    <row r="7" ht="15.6" spans="2:11">
       <c r="B7" s="13" t="s">
         <v>11</v>
       </c>
@@ -3236,7 +3371,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" ht="15.75" spans="2:11">
+    <row r="8" ht="15.6" spans="2:11">
       <c r="B8" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(B6)+D6*1024-1)</f>
         <v>3FFFF</v>
@@ -3251,7 +3386,7 @@
       <c r="J8" s="63"/>
       <c r="K8" s="52"/>
     </row>
-    <row r="9" ht="15.75" spans="2:11">
+    <row r="9" ht="15.6" spans="2:11">
       <c r="B9" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(B8)+1)</f>
         <v>40000</v>
@@ -3274,7 +3409,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" ht="15.75" spans="2:11">
+    <row r="10" ht="15.6" spans="2:11">
       <c r="B10" s="13" t="s">
         <v>11</v>
       </c>
@@ -3288,7 +3423,7 @@
       <c r="J10" s="71"/>
       <c r="K10" s="52"/>
     </row>
-    <row r="11" ht="15.75" spans="2:11">
+    <row r="11" ht="15.6" spans="2:11">
       <c r="B11" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(B9)+D9*1024-1)</f>
         <v>7EFFF</v>
@@ -3307,7 +3442,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" ht="15.75" spans="2:11">
+    <row r="12" ht="15.6" spans="2:11">
       <c r="B12" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(B11)+1)</f>
         <v>7F000</v>
@@ -3328,7 +3463,7 @@
       <c r="J12" s="75"/>
       <c r="K12" s="52"/>
     </row>
-    <row r="13" ht="15.75" spans="2:11">
+    <row r="13" ht="15.6" spans="2:11">
       <c r="B13" s="13" t="s">
         <v>11</v>
       </c>
@@ -3346,7 +3481,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" ht="15.75" spans="2:11">
+    <row r="14" ht="15.6" spans="2:11">
       <c r="B14" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(B12)+D12*1024-1)</f>
         <v>7FFFF</v>
@@ -3386,7 +3521,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" ht="15.75" spans="2:11">
+    <row r="16" ht="15.6" spans="2:11">
       <c r="B16" s="13" t="s">
         <v>11</v>
       </c>
@@ -3400,7 +3535,7 @@
       <c r="J16" s="88"/>
       <c r="K16" s="52"/>
     </row>
-    <row r="17" ht="15.75" spans="2:11">
+    <row r="17" ht="15.6" spans="2:11">
       <c r="B17" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(B15)+D15*1024-1)</f>
         <v>B3FFF</v>
@@ -3419,7 +3554,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" ht="15.75" spans="2:11">
+    <row r="18" ht="15.6" spans="2:11">
       <c r="B18" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(B17)+1)</f>
         <v>B4000</v>
@@ -3440,7 +3575,7 @@
       <c r="J18" s="92"/>
       <c r="K18" s="52"/>
     </row>
-    <row r="19" ht="15.75" spans="2:11">
+    <row r="19" ht="15.6" spans="2:11">
       <c r="B19" s="13" t="s">
         <v>11</v>
       </c>
@@ -3458,7 +3593,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" ht="15.75" spans="2:11">
+    <row r="20" ht="15.6" spans="2:11">
       <c r="B20" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(B18)+D18*1024-1)</f>
         <v>D1FFF</v>
@@ -3473,7 +3608,7 @@
       <c r="J20" s="96"/>
       <c r="K20" s="52"/>
     </row>
-    <row r="21" ht="15.75" spans="2:11">
+    <row r="21" ht="15.6" spans="2:11">
       <c r="B21" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(B20)+1)</f>
         <v>D2000</v>
@@ -3498,7 +3633,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" ht="15.75" spans="2:11">
+    <row r="22" ht="15.6" spans="2:11">
       <c r="B22" s="13" t="s">
         <v>11</v>
       </c>
@@ -3512,7 +3647,7 @@
       <c r="J22" s="100"/>
       <c r="K22" s="52"/>
     </row>
-    <row r="23" ht="15.75" spans="2:11">
+    <row r="23" ht="15.6" spans="2:11">
       <c r="B23" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(B21)+D21*1024-1)</f>
         <v>D7FFF</v>
@@ -3531,7 +3666,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" ht="15.75" spans="2:11">
+    <row r="24" ht="15.6" spans="2:11">
       <c r="B24" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(B23)+1)</f>
         <v>D8000</v>
@@ -3552,7 +3687,7 @@
       <c r="J24" s="104"/>
       <c r="K24" s="52"/>
     </row>
-    <row r="25" ht="15.75" spans="2:11">
+    <row r="25" ht="15.6" spans="2:11">
       <c r="B25" s="13" t="s">
         <v>11</v>
       </c>
@@ -3570,7 +3705,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" ht="15.75" spans="2:11">
+    <row r="26" ht="15.6" spans="2:11">
       <c r="B26" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(B24)+D24*1024-1)</f>
         <v>F9FFF</v>
@@ -3610,7 +3745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" ht="15.75" spans="2:11">
+    <row r="28" ht="15.6" spans="2:11">
       <c r="B28" s="13" t="s">
         <v>11</v>
       </c>
@@ -3624,7 +3759,7 @@
       <c r="J28" s="113"/>
       <c r="K28" s="52"/>
     </row>
-    <row r="29" ht="15.75" spans="2:11">
+    <row r="29" ht="15.6" spans="2:11">
       <c r="B29" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(B27)+D27*1024-1)</f>
         <v>FCFFF</v>
@@ -3697,7 +3832,7 @@
       <c r="J32" s="127"/>
       <c r="K32" s="52"/>
     </row>
-    <row r="33" ht="15.75" spans="2:11">
+    <row r="33" ht="15.6" spans="2:11">
       <c r="B33" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(B32)+1)</f>
         <v>FE000</v>
@@ -3722,7 +3857,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" ht="15.75" spans="2:11">
+    <row r="34" ht="15.6" spans="2:11">
       <c r="B34" s="13" t="s">
         <v>11</v>
       </c>
@@ -3755,7 +3890,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" ht="15.75" spans="2:11">
+    <row r="36" ht="15.6" spans="2:11">
       <c r="B36" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(B35)+1)</f>
         <v>FF000</v>
@@ -3774,7 +3909,7 @@
       <c r="J36" s="119"/>
       <c r="K36" s="52"/>
     </row>
-    <row r="37" ht="15.75" spans="2:11">
+    <row r="37" ht="15.6" spans="2:11">
       <c r="B37" s="13" t="s">
         <v>11</v>
       </c>
@@ -3792,7 +3927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" ht="15.75" spans="2:11">
+    <row r="38" ht="15.6" spans="2:11">
       <c r="B38" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(B36)+D36*1024-1)</f>
         <v>FFFFF</v>
@@ -3807,7 +3942,7 @@
       <c r="J38" s="127"/>
       <c r="K38" s="52"/>
     </row>
-    <row r="39" ht="15.75" spans="9:11">
+    <row r="39" ht="15.6" spans="9:11">
       <c r="I39" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(I38)+1)</f>
         <v>C6000</v>
@@ -3819,7 +3954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" ht="15.75" spans="9:11">
+    <row r="40" ht="15.6" spans="9:11">
       <c r="I40" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(I39)+K39*1024-1)</f>
         <v>C6FFF</v>
@@ -3827,7 +3962,7 @@
       <c r="J40" s="133"/>
       <c r="K40" s="52"/>
     </row>
-    <row r="41" ht="15.75" spans="9:11">
+    <row r="41" ht="15.6" spans="9:11">
       <c r="I41" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(I40)+1)</f>
         <v>C7000</v>
@@ -3839,7 +3974,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" ht="15.75" spans="9:11">
+    <row r="42" ht="15.6" spans="9:11">
       <c r="I42" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(I41)+K41*1024-1)</f>
         <v>C7FFF</v>
@@ -3847,7 +3982,7 @@
       <c r="J42" s="50"/>
       <c r="K42" s="52"/>
     </row>
-    <row r="43" ht="15.75" spans="9:11">
+    <row r="43" ht="15.6" spans="9:11">
       <c r="I43" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(I42)+1)</f>
         <v>C8000</v>
@@ -3859,7 +3994,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" ht="15.75" spans="9:11">
+    <row r="44" ht="15.6" spans="9:11">
       <c r="I44" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(I43)+K43*1024-1)</f>
         <v>C8FFF</v>
@@ -3867,7 +4002,7 @@
       <c r="J44" s="147"/>
       <c r="K44" s="52"/>
     </row>
-    <row r="45" ht="15.75" spans="9:11">
+    <row r="45" ht="15.6" spans="9:11">
       <c r="I45" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(I44)+1)</f>
         <v>C9000</v>
@@ -3879,7 +4014,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" ht="15.75" spans="9:11">
+    <row r="46" ht="15.6" spans="9:11">
       <c r="I46" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(I45)+K45*1024-1)</f>
         <v>C9FFF</v>
@@ -3887,7 +4022,7 @@
       <c r="J46" s="55"/>
       <c r="K46" s="52"/>
     </row>
-    <row r="47" ht="15.75" spans="9:11">
+    <row r="47" ht="15.6" spans="9:11">
       <c r="I47" s="9" t="str">
         <f t="shared" ref="I47:I51" si="1">DEC2HEX(HEX2DEC(I46)+1)</f>
         <v>CA000</v>
@@ -3899,7 +4034,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" ht="15.75" spans="9:11">
+    <row r="48" ht="15.6" spans="9:11">
       <c r="I48" s="14" t="str">
         <f t="shared" ref="I48:I52" si="2">DEC2HEX(HEX2DEC(I47)+K47*1024-1)</f>
         <v>CAFFF</v>
@@ -3907,7 +4042,7 @@
       <c r="J48" s="147"/>
       <c r="K48" s="52"/>
     </row>
-    <row r="49" ht="15.75" spans="9:11">
+    <row r="49" ht="15.6" spans="9:11">
       <c r="I49" s="9" t="str">
         <f t="shared" si="1"/>
         <v>CB000</v>
@@ -3919,7 +4054,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" ht="15.75" spans="9:11">
+    <row r="50" ht="15.6" spans="9:11">
       <c r="I50" s="14" t="str">
         <f t="shared" si="2"/>
         <v>CBFFF</v>
@@ -3927,7 +4062,7 @@
       <c r="J50" s="63"/>
       <c r="K50" s="52"/>
     </row>
-    <row r="51" ht="15.75" spans="9:11">
+    <row r="51" ht="15.6" spans="9:11">
       <c r="I51" s="9" t="str">
         <f t="shared" si="1"/>
         <v>CC000</v>
@@ -3939,7 +4074,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" ht="15.75" spans="9:11">
+    <row r="52" ht="15.6" spans="9:11">
       <c r="I52" s="14" t="str">
         <f t="shared" si="2"/>
         <v>D1FFF</v>
@@ -4058,24 +4193,24 @@
   <sheetPr/>
   <dimension ref="B1:N43"/>
   <sheetViews>
-    <sheetView zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="9.25" style="6" customWidth="1"/>
-    <col min="3" max="3" width="30.625" customWidth="1"/>
+    <col min="3" max="3" width="30.6296296296296" customWidth="1"/>
     <col min="4" max="4" width="9.75" customWidth="1"/>
-    <col min="5" max="5" width="32.425" customWidth="1"/>
-    <col min="6" max="6" width="5.625" customWidth="1"/>
+    <col min="5" max="5" width="32.4259259259259" customWidth="1"/>
+    <col min="6" max="6" width="5.62962962962963" customWidth="1"/>
     <col min="7" max="7" width="5" customWidth="1"/>
-    <col min="8" max="8" width="9.875" style="6" customWidth="1"/>
-    <col min="9" max="9" width="35.1333333333333" customWidth="1"/>
-    <col min="10" max="10" width="10.375" customWidth="1"/>
-    <col min="12" max="12" width="9.11666666666667" customWidth="1"/>
-    <col min="13" max="13" width="31.125" customWidth="1"/>
+    <col min="8" max="8" width="9.87962962962963" style="6" customWidth="1"/>
+    <col min="9" max="9" width="35.1296296296296" customWidth="1"/>
+    <col min="10" max="10" width="10.3796296296296" customWidth="1"/>
+    <col min="12" max="12" width="9.12037037037037" customWidth="1"/>
+    <col min="13" max="13" width="31.1296296296296" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="39" customHeight="1" spans="2:14">
@@ -4128,7 +4263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" ht="15.75" spans="2:14">
+    <row r="3" ht="15.6" spans="2:14">
       <c r="B3" s="184" t="s">
         <v>7</v>
       </c>
@@ -4136,11 +4271,11 @@
         <v>8</v>
       </c>
       <c r="D3" s="11">
-        <v>440</v>
+        <v>384</v>
       </c>
       <c r="E3" s="161"/>
-      <c r="H3" s="9">
-        <v>70000</v>
+      <c r="H3" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="I3" s="47" t="s">
         <v>9</v>
@@ -4149,7 +4284,7 @@
         <v>4</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M3" s="131" t="s">
         <v>50</v>
@@ -4158,37 +4293,34 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" ht="15.75" spans="2:14">
+    <row r="4" ht="15.6" spans="2:14">
       <c r="B4" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="21"/>
       <c r="D4" s="11"/>
       <c r="E4" s="162"/>
-      <c r="H4" s="14" t="str">
-        <f t="shared" ref="H4:H8" si="0">DEC2HEX(HEX2DEC(H3)+J3*1024-1)</f>
-        <v>70FFF</v>
+      <c r="H4" s="14" t="s">
+        <v>77</v>
       </c>
       <c r="I4" s="50"/>
       <c r="J4" s="52"/>
       <c r="L4" s="14" t="str">
-        <f t="shared" ref="L4:L8" si="1">DEC2HEX(HEX2DEC(L3)+N3*1024-1)</f>
+        <f t="shared" ref="L4:L8" si="0">DEC2HEX(HEX2DEC(L3)+N3*1024-1)</f>
         <v>F0FFF</v>
       </c>
       <c r="M4" s="133"/>
       <c r="N4" s="52"/>
     </row>
-    <row r="5" ht="15.75" spans="2:14">
-      <c r="B5" s="14" t="str">
-        <f>DEC2HEX(HEX2DEC(B3)+D3*1024-1)</f>
-        <v>6DFFF</v>
+    <row r="5" ht="15.6" spans="2:14">
+      <c r="B5" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="C5" s="21"/>
       <c r="D5" s="11"/>
       <c r="E5" s="162"/>
-      <c r="H5" s="9" t="str">
-        <f t="shared" ref="H5:H9" si="2">DEC2HEX(HEX2DEC(H4)+1)</f>
-        <v>71000</v>
+      <c r="H5" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="I5" s="53" t="s">
         <v>12</v>
@@ -4197,7 +4329,7 @@
         <v>4</v>
       </c>
       <c r="L5" s="9" t="str">
-        <f t="shared" ref="L5:L9" si="3">DEC2HEX(HEX2DEC(L4)+1)</f>
+        <f t="shared" ref="L5:L9" si="1">DEC2HEX(HEX2DEC(L4)+1)</f>
         <v>F1000</v>
       </c>
       <c r="M5" s="135" t="s">
@@ -4207,43 +4339,40 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" ht="15.75" spans="2:14">
-      <c r="B6" s="9" t="str">
-        <f>DEC2HEX(HEX2DEC(B5)+1)</f>
-        <v>6E000</v>
+    <row r="6" ht="15.6" spans="2:14">
+      <c r="B6" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="C6" s="57" t="s">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="D6" s="25">
-        <v>72</v>
+        <v>128</v>
       </c>
       <c r="E6" s="166" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>71FFF</v>
+        <v>82</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>83</v>
       </c>
       <c r="I6" s="55"/>
       <c r="J6" s="52"/>
       <c r="L6" s="14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>F1FFF</v>
       </c>
       <c r="M6" s="137"/>
       <c r="N6" s="52"/>
     </row>
-    <row r="7" ht="15.75" spans="2:14">
+    <row r="7" ht="15.6" spans="2:14">
       <c r="B7" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="61"/>
       <c r="D7" s="29"/>
       <c r="E7" s="167"/>
-      <c r="H7" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>72000</v>
+      <c r="H7" s="9" t="s">
+        <v>84</v>
       </c>
       <c r="I7" s="59" t="s">
         <v>16</v>
@@ -4252,7 +4381,7 @@
         <v>4</v>
       </c>
       <c r="L7" s="9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>F2000</v>
       </c>
       <c r="M7" s="141" t="s">
@@ -4262,42 +4391,38 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" ht="15.75" spans="2:14">
-      <c r="B8" s="14" t="str">
-        <f>DEC2HEX(HEX2DEC(B6)+D6*1024-1)</f>
-        <v>7FFFF</v>
+    <row r="8" ht="15.6" spans="2:14">
+      <c r="B8" s="14" t="s">
+        <v>85</v>
       </c>
       <c r="C8" s="65"/>
       <c r="D8" s="33"/>
       <c r="E8" s="170"/>
-      <c r="H8" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>72FFF</v>
+      <c r="H8" s="14" t="s">
+        <v>86</v>
       </c>
       <c r="I8" s="63"/>
       <c r="J8" s="52"/>
       <c r="L8" s="14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>F2FFF</v>
       </c>
       <c r="M8" s="145"/>
       <c r="N8" s="52"/>
     </row>
-    <row r="9" ht="15.75" spans="2:14">
-      <c r="B9" s="9" t="str">
-        <f>DEC2HEX(HEX2DEC(B8)+1)</f>
-        <v>80000</v>
+    <row r="9" ht="15.6" spans="2:14">
+      <c r="B9" s="9" t="s">
+        <v>87</v>
       </c>
       <c r="C9" s="21" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="11">
-        <v>440</v>
+        <v>384</v>
       </c>
       <c r="E9" s="171"/>
-      <c r="H9" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>73000</v>
+      <c r="H9" s="9" t="s">
+        <v>88</v>
       </c>
       <c r="I9" s="67" t="s">
         <v>19</v>
@@ -4306,47 +4431,44 @@
         <v>4</v>
       </c>
       <c r="L9" s="9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>F3000</v>
       </c>
       <c r="M9" s="149" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="N9" s="49">
         <v>4</v>
       </c>
     </row>
-    <row r="10" ht="15.75" spans="2:14">
+    <row r="10" ht="15.6" spans="2:14">
       <c r="B10" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="21"/>
       <c r="D10" s="11"/>
       <c r="E10" s="167"/>
-      <c r="H10" s="14" t="str">
-        <f t="shared" ref="H10:H14" si="4">DEC2HEX(HEX2DEC(H9)+J9*1024-1)</f>
-        <v>73FFF</v>
+      <c r="H10" s="14" t="s">
+        <v>89</v>
       </c>
       <c r="I10" s="71"/>
       <c r="J10" s="52"/>
       <c r="L10" s="14" t="str">
-        <f t="shared" ref="L10:L14" si="5">DEC2HEX(HEX2DEC(L9)+N9*1024-1)</f>
+        <f t="shared" ref="L10:L14" si="2">DEC2HEX(HEX2DEC(L9)+N9*1024-1)</f>
         <v>F3FFF</v>
       </c>
       <c r="M10" s="151"/>
       <c r="N10" s="52"/>
     </row>
-    <row r="11" ht="15.75" spans="2:14">
-      <c r="B11" s="14" t="str">
-        <f>DEC2HEX(HEX2DEC(B9)+D9*1024-1)</f>
-        <v>EDFFF</v>
+    <row r="11" ht="15.6" spans="2:14">
+      <c r="B11" s="14" t="s">
+        <v>90</v>
       </c>
       <c r="C11" s="21"/>
       <c r="D11" s="11"/>
       <c r="E11" s="170"/>
-      <c r="H11" s="9" t="str">
-        <f t="shared" ref="H11:H15" si="6">DEC2HEX(HEX2DEC(H10)+1)</f>
-        <v>74000</v>
+      <c r="H11" s="9" t="s">
+        <v>91</v>
       </c>
       <c r="I11" s="73" t="s">
         <v>21</v>
@@ -4365,43 +4487,40 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" ht="15.75" spans="2:14">
-      <c r="B12" s="9" t="str">
-        <f>DEC2HEX(HEX2DEC(B11)+1)</f>
-        <v>EE000</v>
+    <row r="12" ht="15.6" spans="2:14">
+      <c r="B12" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="C12" s="57" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D12" s="25">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="E12" s="166" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="14" t="str">
-        <f t="shared" si="4"/>
-        <v>74FFF</v>
+      <c r="H12" s="14" t="s">
+        <v>92</v>
       </c>
       <c r="I12" s="75"/>
       <c r="J12" s="52"/>
       <c r="L12" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>F4FFF</v>
       </c>
       <c r="M12" s="151"/>
       <c r="N12" s="52"/>
     </row>
-    <row r="13" ht="15.75" spans="2:14">
+    <row r="13" ht="15.6" spans="2:14">
       <c r="B13" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="61"/>
       <c r="D13" s="29"/>
       <c r="E13" s="167"/>
-      <c r="H13" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>75000</v>
+      <c r="H13" s="9" t="s">
+        <v>93</v>
       </c>
       <c r="I13" s="79" t="s">
         <v>24</v>
@@ -4420,44 +4539,40 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" ht="15.75" spans="2:14">
-      <c r="B14" s="14" t="str">
-        <f>DEC2HEX(HEX2DEC(B12)+D12*1024-1)</f>
-        <v>F5FFF</v>
+    <row r="14" ht="15.6" spans="2:14">
+      <c r="B14" s="14" t="s">
+        <v>94</v>
       </c>
       <c r="C14" s="65"/>
       <c r="D14" s="33"/>
       <c r="E14" s="170"/>
-      <c r="H14" s="14" t="str">
-        <f t="shared" si="4"/>
-        <v>75FFF</v>
+      <c r="H14" s="14" t="s">
+        <v>95</v>
       </c>
       <c r="I14" s="65"/>
       <c r="J14" s="52"/>
       <c r="L14" s="14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>F5FFF</v>
       </c>
       <c r="M14" s="155"/>
       <c r="N14" s="52"/>
     </row>
     <row r="15" ht="15.75" customHeight="1" spans="2:10">
-      <c r="B15" s="9" t="str">
-        <f>DEC2HEX(HEX2DEC(B14)+1)</f>
-        <v>F6000</v>
-      </c>
-      <c r="C15" s="86" t="s">
-        <v>36</v>
+      <c r="B15" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="57" t="s">
+        <v>23</v>
       </c>
       <c r="D15" s="25">
-        <v>32</v>
-      </c>
-      <c r="E15" s="171" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>76000</v>
+        <v>24</v>
+      </c>
+      <c r="E15" s="166" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>96</v>
       </c>
       <c r="I15" s="84" t="s">
         <v>27</v>
@@ -4466,31 +4581,28 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" ht="15.75" spans="2:10">
+    <row r="16" ht="15.6" spans="2:10">
       <c r="B16" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="90"/>
+      <c r="C16" s="61"/>
       <c r="D16" s="29"/>
       <c r="E16" s="167"/>
-      <c r="H16" s="14" t="str">
-        <f t="shared" ref="H16:H20" si="7">DEC2HEX(HEX2DEC(H15)+J15*1024-1)</f>
-        <v>76FFF</v>
+      <c r="H16" s="14" t="s">
+        <v>97</v>
       </c>
       <c r="I16" s="88"/>
       <c r="J16" s="52"/>
     </row>
-    <row r="17" ht="15.75" spans="2:10">
-      <c r="B17" s="14" t="str">
-        <f>DEC2HEX(HEX2DEC(B15)+D15*1024-1)</f>
-        <v>FDFFF</v>
-      </c>
-      <c r="C17" s="92"/>
+    <row r="17" ht="15.6" spans="2:10">
+      <c r="B17" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="65"/>
       <c r="D17" s="33"/>
       <c r="E17" s="170"/>
-      <c r="H17" s="9" t="str">
-        <f t="shared" ref="H17:H21" si="8">DEC2HEX(HEX2DEC(H16)+1)</f>
-        <v>77000</v>
+      <c r="H17" s="9" t="s">
+        <v>99</v>
       </c>
       <c r="I17" s="86" t="s">
         <v>28</v>
@@ -4499,37 +4611,34 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" ht="15.75" spans="2:10">
-      <c r="B18" s="9" t="str">
-        <f>DEC2HEX(HEX2DEC(B17)+1)</f>
-        <v>FE000</v>
-      </c>
-      <c r="C18" s="180" t="s">
-        <v>77</v>
+    <row r="18" ht="15.6" spans="2:10">
+      <c r="B18" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="86" t="s">
+        <v>36</v>
       </c>
       <c r="D18" s="25">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="E18" s="171" t="s">
-        <v>31</v>
-      </c>
-      <c r="H18" s="14" t="str">
-        <f t="shared" si="7"/>
-        <v>77FFF</v>
+        <v>37</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>101</v>
       </c>
       <c r="I18" s="92"/>
       <c r="J18" s="52"/>
     </row>
-    <row r="19" ht="15.75" spans="2:10">
+    <row r="19" ht="15.6" spans="2:10">
       <c r="B19" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="143"/>
+      <c r="C19" s="90"/>
       <c r="D19" s="29"/>
       <c r="E19" s="167"/>
-      <c r="H19" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>78000</v>
+      <c r="H19" s="9" t="s">
+        <v>102</v>
       </c>
       <c r="I19" s="141" t="s">
         <v>17</v>
@@ -4538,36 +4647,34 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" ht="15.75" spans="2:10">
-      <c r="B20" s="14" t="str">
-        <f>DEC2HEX(HEX2DEC(B18)+D21*1024-1)</f>
-        <v>FEFFF</v>
-      </c>
-      <c r="C20" s="147"/>
+    <row r="20" ht="15.6" spans="2:10">
+      <c r="B20" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="92"/>
       <c r="D20" s="33"/>
       <c r="E20" s="170"/>
-      <c r="H20" s="14" t="str">
-        <f t="shared" si="7"/>
-        <v>78FFF</v>
+      <c r="H20" s="14" t="s">
+        <v>104</v>
       </c>
       <c r="I20" s="145"/>
       <c r="J20" s="52"/>
     </row>
-    <row r="21" ht="15.75" spans="2:10">
-      <c r="B21" s="9" t="str">
-        <f>DEC2HEX(HEX2DEC(B20)+1)</f>
-        <v>FF000</v>
-      </c>
-      <c r="C21" s="139" t="s">
-        <v>78</v>
+    <row r="21" ht="15.6" spans="2:10">
+      <c r="B21" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="180" t="s">
+        <v>106</v>
       </c>
       <c r="D21" s="25">
         <v>4</v>
       </c>
-      <c r="E21" s="171"/>
-      <c r="H21" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>79000</v>
+      <c r="E21" s="171" t="s">
+        <v>31</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>107</v>
       </c>
       <c r="I21" s="98" t="s">
         <v>38</v>
@@ -4576,31 +4683,28 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" ht="15.75" spans="2:10">
+    <row r="22" ht="15.6" spans="2:10">
       <c r="B22" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="143"/>
       <c r="D22" s="29"/>
       <c r="E22" s="167"/>
-      <c r="H22" s="14" t="str">
-        <f t="shared" ref="H22:H26" si="9">DEC2HEX(HEX2DEC(H21)+J21*1024-1)</f>
-        <v>79FFF</v>
+      <c r="H22" s="14" t="s">
+        <v>108</v>
       </c>
       <c r="I22" s="100"/>
       <c r="J22" s="52"/>
     </row>
-    <row r="23" ht="15.75" spans="2:10">
-      <c r="B23" s="14" t="str">
-        <f>DEC2HEX(HEX2DEC(B21)+D18*1024-1)</f>
-        <v>FFFFF</v>
+    <row r="23" ht="15.6" spans="2:10">
+      <c r="B23" s="14" t="s">
+        <v>109</v>
       </c>
       <c r="C23" s="147"/>
       <c r="D23" s="33"/>
       <c r="E23" s="170"/>
-      <c r="H23" s="9" t="str">
-        <f t="shared" ref="H23:H27" si="10">DEC2HEX(HEX2DEC(H22)+1)</f>
-        <v>7A000</v>
+      <c r="H23" s="9" t="s">
+        <v>110</v>
       </c>
       <c r="I23" s="102" t="s">
         <v>41</v>
@@ -4609,18 +4713,32 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" ht="15.75" spans="8:10">
-      <c r="H24" s="14" t="str">
-        <f t="shared" si="9"/>
-        <v>7AFFF</v>
+    <row r="24" ht="15.6" spans="2:10">
+      <c r="B24" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" s="139" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" s="25">
+        <v>4</v>
+      </c>
+      <c r="E24" s="171"/>
+      <c r="H24" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="I24" s="104"/>
       <c r="J24" s="52"/>
     </row>
-    <row r="25" ht="15.75" spans="8:10">
-      <c r="H25" s="9" t="str">
-        <f t="shared" si="10"/>
-        <v>7B000</v>
+    <row r="25" ht="15.6" spans="2:10">
+      <c r="B25" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="143"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="167"/>
+      <c r="H25" s="9" t="s">
+        <v>114</v>
       </c>
       <c r="I25" s="106" t="s">
         <v>44</v>
@@ -4629,18 +4747,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" ht="15.75" spans="8:10">
-      <c r="H26" s="14" t="str">
-        <f t="shared" si="9"/>
-        <v>7BFFF</v>
+    <row r="26" ht="15.6" spans="2:10">
+      <c r="B26" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" s="147"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="170"/>
+      <c r="H26" s="14" t="s">
+        <v>116</v>
       </c>
       <c r="I26" s="108"/>
       <c r="J26" s="52"/>
     </row>
     <row r="27" ht="15.75" customHeight="1" spans="8:10">
-      <c r="H27" s="9" t="str">
-        <f t="shared" si="10"/>
-        <v>7C000</v>
+      <c r="H27" s="9" t="s">
+        <v>117</v>
       </c>
       <c r="I27" s="131" t="s">
         <v>10</v>
@@ -4649,18 +4771,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" ht="15.75" spans="8:10">
-      <c r="H28" s="14" t="str">
-        <f t="shared" ref="H28:H32" si="11">DEC2HEX(HEX2DEC(H27)+J27*1024-1)</f>
-        <v>7CFFF</v>
+    <row r="28" ht="15.6" spans="8:10">
+      <c r="H28" s="14" t="s">
+        <v>118</v>
       </c>
       <c r="I28" s="133"/>
       <c r="J28" s="52"/>
     </row>
-    <row r="29" ht="15.75" spans="8:10">
-      <c r="H29" s="9" t="str">
-        <f t="shared" ref="H29:H33" si="12">DEC2HEX(HEX2DEC(H28)+1)</f>
-        <v>7D000</v>
+    <row r="29" ht="15.6" spans="8:10">
+      <c r="H29" s="9" t="s">
+        <v>119</v>
       </c>
       <c r="I29" s="116" t="s">
         <v>13</v>
@@ -4670,17 +4790,15 @@
       </c>
     </row>
     <row r="30" ht="14.25" customHeight="1" spans="8:10">
-      <c r="H30" s="14" t="str">
-        <f t="shared" si="11"/>
-        <v>7DFFF</v>
+      <c r="H30" s="14" t="s">
+        <v>120</v>
       </c>
       <c r="I30" s="119"/>
       <c r="J30" s="52"/>
     </row>
     <row r="31" ht="14.25" customHeight="1" spans="8:10">
-      <c r="H31" s="9" t="str">
-        <f t="shared" si="12"/>
-        <v>7E000</v>
+      <c r="H31" s="9" t="s">
+        <v>121</v>
       </c>
       <c r="I31" s="116" t="s">
         <v>47</v>
@@ -4690,29 +4808,26 @@
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1" spans="8:10">
-      <c r="H32" s="14" t="str">
-        <f t="shared" si="11"/>
-        <v>7EFFF</v>
+      <c r="H32" s="14" t="s">
+        <v>122</v>
       </c>
       <c r="I32" s="119"/>
       <c r="J32" s="52"/>
     </row>
-    <row r="33" ht="15.75" spans="8:10">
-      <c r="H33" s="9" t="str">
-        <f t="shared" si="12"/>
-        <v>7F000</v>
+    <row r="33" ht="15.6" spans="8:10">
+      <c r="H33" s="9" t="s">
+        <v>123</v>
       </c>
       <c r="I33" s="123" t="s">
-        <v>79</v>
+        <v>124</v>
       </c>
       <c r="J33" s="49">
         <v>4</v>
       </c>
     </row>
-    <row r="34" ht="15.75" spans="8:10">
-      <c r="H34" s="14" t="str">
-        <f>DEC2HEX(HEX2DEC(H33)+J33*1024-1)</f>
-        <v>7FFFF</v>
+    <row r="34" ht="15.6" spans="8:10">
+      <c r="H34" s="14" t="s">
+        <v>94</v>
       </c>
       <c r="I34" s="127"/>
       <c r="J34" s="52"/>
@@ -4745,7 +4860,7 @@
       <c r="H43"/>
     </row>
   </sheetData>
-  <mergeCells count="68">
+  <mergeCells count="71">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="L1:N1"/>
@@ -4756,6 +4871,7 @@
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="C18:C20"/>
     <mergeCell ref="C21:C23"/>
+    <mergeCell ref="C24:C26"/>
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="D6:D8"/>
     <mergeCell ref="D9:D11"/>
@@ -4763,6 +4879,7 @@
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="D18:D20"/>
     <mergeCell ref="D21:D23"/>
+    <mergeCell ref="D24:D26"/>
     <mergeCell ref="E3:E5"/>
     <mergeCell ref="E6:E8"/>
     <mergeCell ref="E9:E11"/>
@@ -4770,6 +4887,7 @@
     <mergeCell ref="E15:E17"/>
     <mergeCell ref="E18:E20"/>
     <mergeCell ref="E21:E23"/>
+    <mergeCell ref="E24:E26"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="I7:I8"/>
@@ -4830,7 +4948,7 @@
       <selection activeCell="C26" sqref="C26:C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9.25" style="6" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="27.75" hidden="1" customWidth="1"/>
@@ -4838,21 +4956,21 @@
     <col min="4" max="4" width="9.75" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="28.75" hidden="1" customWidth="1"/>
     <col min="6" max="7" width="9" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="9.875" style="6" customWidth="1"/>
-    <col min="9" max="9" width="31.125" customWidth="1"/>
-    <col min="10" max="10" width="21.875" customWidth="1"/>
+    <col min="8" max="8" width="9.87962962962963" style="6" customWidth="1"/>
+    <col min="9" max="9" width="31.1296296296296" customWidth="1"/>
+    <col min="10" max="10" width="21.8796296296296" customWidth="1"/>
     <col min="11" max="11" width="11.25" customWidth="1"/>
     <col min="13" max="13" width="9.25" style="6" customWidth="1"/>
-    <col min="14" max="14" width="31.125" customWidth="1"/>
-    <col min="15" max="15" width="32.125" customWidth="1"/>
+    <col min="14" max="14" width="31.1296296296296" customWidth="1"/>
+    <col min="15" max="15" width="32.1296296296296" customWidth="1"/>
     <col min="16" max="16" width="9.75" customWidth="1"/>
-    <col min="17" max="17" width="30.875" customWidth="1"/>
-    <col min="18" max="18" width="5.625" customWidth="1"/>
-    <col min="19" max="19" width="4.375" customWidth="1"/>
+    <col min="17" max="17" width="30.8796296296296" customWidth="1"/>
+    <col min="18" max="18" width="5.62962962962963" customWidth="1"/>
+    <col min="19" max="19" width="4.37962962962963" customWidth="1"/>
     <col min="20" max="20" width="5" customWidth="1"/>
-    <col min="21" max="21" width="9.875" style="6" customWidth="1"/>
-    <col min="22" max="22" width="31.125" customWidth="1"/>
-    <col min="23" max="23" width="12.625" customWidth="1"/>
+    <col min="21" max="21" width="9.87962962962963" style="6" customWidth="1"/>
+    <col min="22" max="22" width="31.1296296296296" customWidth="1"/>
+    <col min="23" max="23" width="12.6296296296296" customWidth="1"/>
     <col min="24" max="24" width="11.25" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4868,7 +4986,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>3</v>
@@ -4904,12 +5022,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="15.75" spans="1:24">
+    <row r="2" ht="15.6" spans="1:24">
       <c r="A2" s="184" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>81</v>
+        <v>126</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="11">
@@ -4931,28 +5049,28 @@
         <v>7</v>
       </c>
       <c r="N2" s="21" t="s">
-        <v>82</v>
+        <v>127</v>
       </c>
       <c r="O2" s="21"/>
       <c r="P2" s="11">
         <v>24</v>
       </c>
       <c r="Q2" s="161" t="s">
-        <v>83</v>
+        <v>128</v>
       </c>
       <c r="U2" s="184" t="str">
         <f>M23</f>
         <v>26000</v>
       </c>
       <c r="V2" s="47" t="s">
-        <v>84</v>
+        <v>129</v>
       </c>
       <c r="W2" s="48"/>
       <c r="X2" s="49">
         <v>8</v>
       </c>
     </row>
-    <row r="3" ht="15.75" spans="1:24">
+    <row r="3" ht="15.6" spans="1:24">
       <c r="A3" s="13" t="s">
         <v>11</v>
       </c>
@@ -4981,7 +5099,7 @@
       <c r="W3" s="164"/>
       <c r="X3" s="165"/>
     </row>
-    <row r="4" ht="15.75" spans="1:24">
+    <row r="4" ht="15.6" spans="1:24">
       <c r="A4" s="185" t="str">
         <f>DEC2HEX(HEX2DEC(A2)+D2*1024-1)</f>
         <v>2FFFF</v>
@@ -5017,13 +5135,13 @@
       <c r="W4" s="51"/>
       <c r="X4" s="52"/>
     </row>
-    <row r="5" ht="15.75" spans="1:24">
+    <row r="5" ht="15.6" spans="1:24">
       <c r="A5" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(A4)+1)</f>
         <v>30000</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>85</v>
+        <v>130</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="11">
@@ -5042,28 +5160,28 @@
         <v>6000</v>
       </c>
       <c r="N5" s="57" t="s">
-        <v>86</v>
+        <v>131</v>
       </c>
       <c r="O5" s="58"/>
       <c r="P5" s="25">
         <v>4</v>
       </c>
       <c r="Q5" s="166" t="s">
-        <v>87</v>
+        <v>132</v>
       </c>
       <c r="U5" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(U4)+1)</f>
         <v>28000</v>
       </c>
       <c r="V5" s="53" t="s">
-        <v>88</v>
+        <v>133</v>
       </c>
       <c r="W5" s="54"/>
       <c r="X5" s="49">
         <v>8</v>
       </c>
     </row>
-    <row r="6" ht="15.75" spans="1:24">
+    <row r="6" ht="15.6" spans="1:24">
       <c r="A6" s="13" t="s">
         <v>11</v>
       </c>
@@ -5096,7 +5214,7 @@
       <c r="W6" s="169"/>
       <c r="X6" s="165"/>
     </row>
-    <row r="7" ht="15.75" spans="1:24">
+    <row r="7" ht="15.6" spans="1:24">
       <c r="A7" s="14" t="e">
         <f>DEC2HEX(HEX2DEC(#REF!)+#REF!*1024-1)</f>
         <v>#REF!</v>
@@ -5128,13 +5246,13 @@
       <c r="W7" s="56"/>
       <c r="X7" s="52"/>
     </row>
-    <row r="8" ht="15.75" spans="1:24">
+    <row r="8" ht="15.6" spans="1:24">
       <c r="A8" s="9" t="e">
         <f t="shared" ref="A8" si="1">DEC2HEX(HEX2DEC(A7)+1)</f>
         <v>#REF!</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>89</v>
+        <v>134</v>
       </c>
       <c r="C8" s="20"/>
       <c r="D8" s="11">
@@ -5157,28 +5275,28 @@
         <v>7000</v>
       </c>
       <c r="N8" s="69" t="s">
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="O8" s="70"/>
       <c r="P8" s="11">
         <v>4</v>
       </c>
       <c r="Q8" s="171" t="s">
-        <v>91</v>
+        <v>136</v>
       </c>
       <c r="U8" s="9" t="str">
         <f t="shared" ref="U8" si="4">DEC2HEX(HEX2DEC(U7)+1)</f>
         <v>2A000</v>
       </c>
       <c r="V8" s="59" t="s">
-        <v>92</v>
+        <v>137</v>
       </c>
       <c r="W8" s="60"/>
       <c r="X8" s="49">
         <v>8</v>
       </c>
     </row>
-    <row r="9" ht="15.75" spans="1:24">
+    <row r="9" ht="15.6" spans="1:24">
       <c r="A9" s="13" t="s">
         <v>11</v>
       </c>
@@ -5207,7 +5325,7 @@
       <c r="W9" s="173"/>
       <c r="X9" s="165"/>
     </row>
-    <row r="10" ht="15.75" spans="1:24">
+    <row r="10" ht="15.6" spans="1:24">
       <c r="A10" s="14" t="e">
         <f t="shared" ref="A10" si="5">DEC2HEX(HEX2DEC(A8)+D8*1024-1)</f>
         <v>#REF!</v>
@@ -5243,20 +5361,20 @@
       <c r="W10" s="64"/>
       <c r="X10" s="52"/>
     </row>
-    <row r="11" ht="15.75" spans="1:24">
+    <row r="11" ht="15.6" spans="1:24">
       <c r="A11" s="9" t="e">
         <f t="shared" ref="A11" si="8">DEC2HEX(HEX2DEC(A10)+1)</f>
         <v>#REF!</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>93</v>
+        <v>138</v>
       </c>
       <c r="C11" s="21"/>
       <c r="D11" s="11">
         <v>128</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
       <c r="H11" s="14" t="str">
         <f>DEC2HEX(HEX2DEC(H10)+K10*1024-1)</f>
@@ -5270,28 +5388,28 @@
         <v>8000</v>
       </c>
       <c r="N11" s="77" t="s">
-        <v>95</v>
+        <v>140</v>
       </c>
       <c r="O11" s="78"/>
       <c r="P11" s="25">
         <v>108</v>
       </c>
       <c r="Q11" s="171" t="s">
-        <v>91</v>
+        <v>136</v>
       </c>
       <c r="U11" s="9" t="str">
         <f t="shared" ref="U11" si="10">DEC2HEX(HEX2DEC(U10)+1)</f>
         <v>2C000</v>
       </c>
       <c r="V11" s="67" t="s">
-        <v>96</v>
+        <v>141</v>
       </c>
       <c r="W11" s="68"/>
       <c r="X11" s="49">
         <v>8</v>
       </c>
     </row>
-    <row r="12" ht="15.75" spans="1:24">
+    <row r="12" ht="15.6" spans="1:24">
       <c r="A12" s="13" t="s">
         <v>11</v>
       </c>
@@ -5324,7 +5442,7 @@
       <c r="W12" s="175"/>
       <c r="X12" s="165"/>
     </row>
-    <row r="13" ht="15.75" spans="1:24">
+    <row r="13" ht="15.6" spans="1:24">
       <c r="A13" s="14" t="e">
         <f t="shared" ref="A13" si="12">DEC2HEX(HEX2DEC(A11)+D11*1024-1)</f>
         <v>#REF!</v>
@@ -5362,10 +5480,10 @@
         <v>#REF!</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>97</v>
+        <v>142</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>98</v>
+        <v>143</v>
       </c>
       <c r="D14" s="11">
         <v>88</v>
@@ -5389,28 +5507,28 @@
         <v>23000</v>
       </c>
       <c r="N14" s="86" t="s">
-        <v>99</v>
+        <v>144</v>
       </c>
       <c r="O14" s="87"/>
       <c r="P14" s="25">
         <v>4</v>
       </c>
       <c r="Q14" s="171" t="s">
-        <v>100</v>
+        <v>145</v>
       </c>
       <c r="U14" s="9" t="str">
         <f t="shared" ref="U14" si="17">DEC2HEX(HEX2DEC(U13)+1)</f>
         <v>2E000</v>
       </c>
       <c r="V14" s="73" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
       <c r="W14" s="74"/>
       <c r="X14" s="49">
         <v>8</v>
       </c>
     </row>
-    <row r="15" ht="15.75" spans="1:24">
+    <row r="15" ht="15.6" spans="1:24">
       <c r="A15" s="13" t="s">
         <v>11</v>
       </c>
@@ -5441,7 +5559,7 @@
       <c r="W15" s="177"/>
       <c r="X15" s="165"/>
     </row>
-    <row r="16" ht="15.75" spans="1:24">
+    <row r="16" ht="15.6" spans="1:24">
       <c r="A16" s="14" t="e">
         <f t="shared" ref="A16" si="18">DEC2HEX(HEX2DEC(A14)+D14*1024-1)</f>
         <v>#REF!</v>
@@ -5479,16 +5597,16 @@
       <c r="W16" s="76"/>
       <c r="X16" s="52"/>
     </row>
-    <row r="17" ht="15.75" spans="1:24">
+    <row r="17" ht="15.6" spans="1:24">
       <c r="A17" s="9" t="e">
         <f t="shared" ref="A17" si="20">DEC2HEX(HEX2DEC(A16)+1)</f>
         <v>#REF!</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>97</v>
+        <v>142</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>99</v>
+        <v>144</v>
       </c>
       <c r="D17" s="11">
         <v>4</v>
@@ -5508,28 +5626,28 @@
         <v>24000</v>
       </c>
       <c r="N17" s="86" t="s">
-        <v>102</v>
+        <v>147</v>
       </c>
       <c r="O17" s="87"/>
       <c r="P17" s="25">
         <v>4</v>
       </c>
       <c r="Q17" s="171" t="s">
-        <v>103</v>
+        <v>148</v>
       </c>
       <c r="U17" s="9" t="str">
         <f t="shared" ref="U17" si="21">DEC2HEX(HEX2DEC(U16)+1)</f>
         <v>30000</v>
       </c>
       <c r="V17" s="79" t="s">
-        <v>104</v>
+        <v>149</v>
       </c>
       <c r="W17" s="58"/>
       <c r="X17" s="49">
         <v>8</v>
       </c>
     </row>
-    <row r="18" ht="15.75" spans="1:24">
+    <row r="18" ht="15.6" spans="1:24">
       <c r="A18" s="13" t="s">
         <v>11</v>
       </c>
@@ -5564,7 +5682,7 @@
       <c r="W18" s="62"/>
       <c r="X18" s="165"/>
     </row>
-    <row r="19" ht="15.75" spans="1:24">
+    <row r="19" ht="15.6" spans="1:24">
       <c r="A19" s="14" t="e">
         <f t="shared" ref="A19" si="23">DEC2HEX(HEX2DEC(A17)+D17*1024-1)</f>
         <v>#REF!</v>
@@ -5598,16 +5716,16 @@
       <c r="W19" s="66"/>
       <c r="X19" s="52"/>
     </row>
-    <row r="20" ht="15.75" spans="1:24">
+    <row r="20" ht="15.6" spans="1:24">
       <c r="A20" s="9" t="e">
         <f t="shared" ref="A20" si="24">DEC2HEX(HEX2DEC(A19)+1)</f>
         <v>#REF!</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>97</v>
+        <v>142</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>105</v>
+        <v>150</v>
       </c>
       <c r="D20" s="25">
         <v>4</v>
@@ -5631,28 +5749,28 @@
         <v>25000</v>
       </c>
       <c r="N20" s="86" t="s">
-        <v>106</v>
+        <v>151</v>
       </c>
       <c r="O20" s="87"/>
       <c r="P20" s="25">
         <v>4</v>
       </c>
       <c r="Q20" s="171" t="s">
-        <v>107</v>
+        <v>152</v>
       </c>
       <c r="U20" s="9" t="str">
         <f t="shared" ref="U20" si="26">DEC2HEX(HEX2DEC(U19)+1)</f>
         <v>32000</v>
       </c>
       <c r="V20" s="84" t="s">
-        <v>108</v>
+        <v>153</v>
       </c>
       <c r="W20" s="85"/>
       <c r="X20" s="49">
         <v>8</v>
       </c>
     </row>
-    <row r="21" ht="15.75" spans="1:24">
+    <row r="21" ht="15.6" spans="1:24">
       <c r="A21" s="13" t="s">
         <v>11</v>
       </c>
@@ -5683,7 +5801,7 @@
       <c r="W21" s="179"/>
       <c r="X21" s="165"/>
     </row>
-    <row r="22" ht="15.75" spans="1:24">
+    <row r="22" ht="15.6" spans="1:24">
       <c r="A22" s="14" t="e">
         <f t="shared" ref="A22" si="27">DEC2HEX(HEX2DEC(A20)+D20*1024-1)</f>
         <v>#REF!</v>
@@ -5721,16 +5839,16 @@
       <c r="W22" s="89"/>
       <c r="X22" s="52"/>
     </row>
-    <row r="23" ht="15.75" spans="1:24">
+    <row r="23" ht="15.6" spans="1:24">
       <c r="A23" s="9" t="e">
         <f>DEC2HEX(HEX2DEC(A22)+1)</f>
         <v>#REF!</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>97</v>
+        <v>142</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>109</v>
+        <v>154</v>
       </c>
       <c r="D23" s="11">
         <v>8</v>
@@ -5750,30 +5868,30 @@
         <v>26000</v>
       </c>
       <c r="N23" s="10" t="s">
-        <v>110</v>
+        <v>155</v>
       </c>
       <c r="O23" s="35" t="s">
-        <v>98</v>
+        <v>143</v>
       </c>
       <c r="P23" s="11">
         <v>88</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>111</v>
+        <v>156</v>
       </c>
       <c r="U23" s="9" t="str">
         <f>DEC2HEX(HEX2DEC(U22)+1)</f>
         <v>34000</v>
       </c>
       <c r="V23" s="86" t="s">
-        <v>112</v>
+        <v>157</v>
       </c>
       <c r="W23" s="87"/>
       <c r="X23" s="49">
         <v>32</v>
       </c>
     </row>
-    <row r="24" ht="15.75" spans="1:24">
+    <row r="24" ht="15.6" spans="1:24">
       <c r="A24" s="13" t="s">
         <v>11</v>
       </c>
@@ -5808,7 +5926,7 @@
       <c r="W24" s="91"/>
       <c r="X24" s="165"/>
     </row>
-    <row r="25" ht="15.75" spans="1:24">
+    <row r="25" ht="15.6" spans="1:24">
       <c r="A25" s="14" t="e">
         <f t="shared" ref="A25" si="30">DEC2HEX(HEX2DEC(A23)+D23*1024-1)</f>
         <v>#REF!</v>
@@ -5848,10 +5966,10 @@
         <v>#REF!</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>97</v>
+        <v>142</v>
       </c>
       <c r="C26" s="35" t="s">
-        <v>113</v>
+        <v>158</v>
       </c>
       <c r="D26" s="11">
         <v>8</v>
@@ -5875,20 +5993,20 @@
         <v>3C000</v>
       </c>
       <c r="N26" s="23" t="s">
-        <v>110</v>
+        <v>155</v>
       </c>
       <c r="O26" s="112" t="s">
-        <v>114</v>
+        <v>159</v>
       </c>
       <c r="P26" s="25">
         <v>8</v>
       </c>
       <c r="Q26" s="171" t="s">
-        <v>115</v>
+        <v>160</v>
       </c>
       <c r="U26"/>
     </row>
-    <row r="27" ht="15.75" spans="1:21">
+    <row r="27" ht="15.6" spans="1:21">
       <c r="A27" s="13" t="s">
         <v>11</v>
       </c>
@@ -5914,7 +6032,7 @@
       <c r="Q27" s="167"/>
       <c r="U27"/>
     </row>
-    <row r="28" ht="15.75" spans="1:21">
+    <row r="28" ht="15.6" spans="1:21">
       <c r="A28" s="14" t="e">
         <f t="shared" ref="A28" si="33">DEC2HEX(HEX2DEC(A26)+D26*1024-1)</f>
         <v>#REF!</v>
@@ -5960,7 +6078,7 @@
         <v>4</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>116</v>
+        <v>161</v>
       </c>
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
@@ -5976,26 +6094,26 @@
         <v>3E000</v>
       </c>
       <c r="N29" s="121" t="s">
-        <v>110</v>
+        <v>155</v>
       </c>
       <c r="O29" s="122" t="s">
-        <v>114</v>
+        <v>159</v>
       </c>
       <c r="P29" s="25">
         <v>8</v>
       </c>
       <c r="Q29" s="171" t="s">
-        <v>117</v>
+        <v>162</v>
       </c>
       <c r="U29"/>
     </row>
-    <row r="30" ht="15.75" spans="1:21">
+    <row r="30" ht="15.6" spans="1:21">
       <c r="A30" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B30" s="37"/>
       <c r="C30" s="24" t="s">
-        <v>118</v>
+        <v>163</v>
       </c>
       <c r="D30" s="11"/>
       <c r="E30" s="12"/>
@@ -6021,7 +6139,7 @@
       <c r="Q30" s="167"/>
       <c r="U30"/>
     </row>
-    <row r="31" ht="15.75" spans="1:21">
+    <row r="31" ht="15.6" spans="1:21">
       <c r="A31" s="14" t="e">
         <f t="shared" ref="A31" si="36">DEC2HEX(HEX2DEC(A29)+D29*1024-1)</f>
         <v>#REF!</v>
@@ -6055,16 +6173,16 @@
         <v>#REF!</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>119</v>
+        <v>164</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>120</v>
+        <v>165</v>
       </c>
       <c r="D32" s="11">
         <v>4</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>121</v>
+        <v>166</v>
       </c>
       <c r="F32" s="22"/>
       <c r="G32" s="22"/>
@@ -6084,18 +6202,18 @@
         <v>40000</v>
       </c>
       <c r="N32" s="39" t="s">
-        <v>122</v>
+        <v>167</v>
       </c>
       <c r="O32" s="40"/>
       <c r="P32" s="25">
         <v>256</v>
       </c>
       <c r="Q32" s="171" t="s">
-        <v>122</v>
+        <v>167</v>
       </c>
       <c r="U32"/>
     </row>
-    <row r="33" ht="15.75" spans="1:21">
+    <row r="33" ht="15.6" spans="1:21">
       <c r="A33" s="13" t="s">
         <v>11</v>
       </c>
@@ -6121,7 +6239,7 @@
       <c r="Q33" s="167"/>
       <c r="U33"/>
     </row>
-    <row r="34" ht="15.75" spans="1:21">
+    <row r="34" ht="15.6" spans="1:21">
       <c r="A34" s="14" t="e">
         <f t="shared" ref="A34" si="40">DEC2HEX(HEX2DEC(A32)+D32*1024-1)</f>
         <v>#REF!</v>
@@ -6153,13 +6271,13 @@
       <c r="Q34" s="170"/>
       <c r="U34"/>
     </row>
-    <row r="35" ht="15.75" spans="1:21">
+    <row r="35" ht="15.6" spans="1:21">
       <c r="A35" s="9" t="e">
         <f t="shared" ref="A35" si="41">DEC2HEX(HEX2DEC(A34)+1)</f>
         <v>#REF!</v>
       </c>
       <c r="B35" s="39" t="s">
-        <v>123</v>
+        <v>168</v>
       </c>
       <c r="C35" s="40"/>
       <c r="D35" s="25">
@@ -6178,18 +6296,18 @@
         <v>80000</v>
       </c>
       <c r="N35" s="139" t="s">
-        <v>124</v>
+        <v>169</v>
       </c>
       <c r="O35" s="140"/>
       <c r="P35" s="11">
         <v>256</v>
       </c>
       <c r="Q35" s="3" t="s">
-        <v>125</v>
+        <v>170</v>
       </c>
       <c r="U35"/>
     </row>
-    <row r="36" ht="15.75" spans="1:21">
+    <row r="36" ht="15.6" spans="1:21">
       <c r="A36" s="13" t="s">
         <v>11</v>
       </c>
@@ -6217,7 +6335,7 @@
       <c r="Q36" s="3"/>
       <c r="U36"/>
     </row>
-    <row r="37" ht="15.75" spans="1:21">
+    <row r="37" ht="15.6" spans="1:21">
       <c r="A37" s="14" t="e">
         <f t="shared" ref="A37" si="43">DEC2HEX(HEX2DEC(A35)+D35*1024-1)</f>
         <v>#REF!</v>
@@ -6243,13 +6361,13 @@
       <c r="Q37" s="3"/>
       <c r="U37"/>
     </row>
-    <row r="38" ht="15.75" spans="1:21">
+    <row r="38" ht="15.6" spans="1:21">
       <c r="A38" s="9" t="e">
         <f t="shared" ref="A38" si="45">DEC2HEX(HEX2DEC(A37)+1)</f>
         <v>#REF!</v>
       </c>
       <c r="B38" s="45" t="s">
-        <v>126</v>
+        <v>171</v>
       </c>
       <c r="C38" s="46"/>
       <c r="D38" s="11">
@@ -6272,18 +6390,18 @@
         <v>C0000</v>
       </c>
       <c r="N38" s="19" t="s">
-        <v>127</v>
+        <v>172</v>
       </c>
       <c r="O38" s="19"/>
       <c r="P38" s="11">
         <v>248</v>
       </c>
       <c r="Q38" s="3" t="s">
-        <v>125</v>
+        <v>170</v>
       </c>
       <c r="U38"/>
     </row>
-    <row r="39" ht="15.75" spans="1:21">
+    <row r="39" ht="15.6" spans="1:21">
       <c r="A39" s="13" t="s">
         <v>11</v>
       </c>
@@ -6307,7 +6425,7 @@
       <c r="Q39" s="3"/>
       <c r="U39"/>
     </row>
-    <row r="40" ht="15.75" spans="1:21">
+    <row r="40" ht="15.6" spans="1:21">
       <c r="A40" s="14" t="e">
         <f t="shared" ref="A40" si="47">DEC2HEX(HEX2DEC(A38)+D38*1024-1)</f>
         <v>#REF!</v>
@@ -6337,7 +6455,7 @@
       <c r="Q40" s="3"/>
       <c r="U40"/>
     </row>
-    <row r="41" ht="15.75" spans="8:21">
+    <row r="41" ht="15.6" spans="8:21">
       <c r="H41" s="14" t="str">
         <f t="shared" ref="H41" si="48">DEC2HEX(HEX2DEC(H40)+K40*1024-1)</f>
         <v>39FFF</v>
@@ -6350,24 +6468,24 @@
         <v>FE000</v>
       </c>
       <c r="N41" s="57" t="s">
-        <v>128</v>
+        <v>173</v>
       </c>
       <c r="O41" s="58"/>
       <c r="P41" s="25">
         <v>4</v>
       </c>
       <c r="Q41" s="166" t="s">
-        <v>129</v>
+        <v>174</v>
       </c>
       <c r="U41"/>
     </row>
-    <row r="42" ht="15.75" spans="8:21">
+    <row r="42" ht="15.6" spans="8:21">
       <c r="H42" s="9" t="str">
         <f t="shared" si="34"/>
         <v>3A000</v>
       </c>
       <c r="I42" s="157" t="s">
-        <v>130</v>
+        <v>175</v>
       </c>
       <c r="J42" s="158"/>
       <c r="K42" s="49">
@@ -6382,7 +6500,7 @@
       <c r="Q42" s="167"/>
       <c r="U42"/>
     </row>
-    <row r="43" ht="15.75" spans="8:21">
+    <row r="43" ht="15.6" spans="8:21">
       <c r="H43" s="14" t="str">
         <f t="shared" ref="H43" si="49">DEC2HEX(HEX2DEC(H42)+K42*1024-1)</f>
         <v>3AFFF</v>
@@ -6400,25 +6518,25 @@
       <c r="Q43" s="170"/>
       <c r="U43"/>
     </row>
-    <row r="44" ht="15.75" spans="8:21">
+    <row r="44" ht="15.6" spans="8:21">
       <c r="H44"/>
       <c r="M44" s="9" t="str">
         <f t="shared" si="16"/>
         <v>FF000</v>
       </c>
       <c r="N44" s="69" t="s">
-        <v>131</v>
+        <v>176</v>
       </c>
       <c r="O44" s="70"/>
       <c r="P44" s="11">
         <v>4</v>
       </c>
       <c r="Q44" s="166" t="s">
-        <v>132</v>
+        <v>177</v>
       </c>
       <c r="U44"/>
     </row>
-    <row r="45" ht="15.75" spans="8:21">
+    <row r="45" ht="15.6" spans="8:21">
       <c r="H45"/>
       <c r="M45" s="13" t="s">
         <v>11</v>
@@ -6429,7 +6547,7 @@
       <c r="Q45" s="167"/>
       <c r="U45"/>
     </row>
-    <row r="46" ht="15.75" spans="13:21">
+    <row r="46" ht="15.6" spans="13:21">
       <c r="M46" s="14" t="str">
         <f t="shared" si="19"/>
         <v>FFFFF</v>
@@ -6648,16 +6766,16 @@
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
-    <col min="2" max="2" width="19.125" customWidth="1"/>
+    <col min="2" max="2" width="19.1296296296296" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>133</v>
+        <v>178</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -6667,7 +6785,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>134</v>
+        <v>179</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -6679,7 +6797,7 @@
     <row r="3" spans="1:7">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -6699,7 +6817,7 @@
     <row r="5" spans="1:7">
       <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
-        <v>136</v>
+        <v>181</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -6719,7 +6837,7 @@
     <row r="7" spans="1:7">
       <c r="A7" s="1"/>
       <c r="B7" s="3" t="s">
-        <v>137</v>
+        <v>182</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -6748,7 +6866,7 @@
     <row r="10" spans="1:7">
       <c r="A10" s="1"/>
       <c r="B10" s="3" t="s">
-        <v>138</v>
+        <v>183</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -6767,7 +6885,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
-        <v>139</v>
+        <v>184</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="1"/>
@@ -6779,7 +6897,7 @@
     <row r="13" spans="1:7">
       <c r="A13" s="2"/>
       <c r="B13" s="3" t="s">
-        <v>140</v>
+        <v>185</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -6808,7 +6926,7 @@
     <row r="16" spans="1:7">
       <c r="A16" s="1"/>
       <c r="B16" s="5" t="s">
-        <v>141</v>
+        <v>186</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -6837,7 +6955,7 @@
     <row r="19" spans="1:7">
       <c r="A19" s="1"/>
       <c r="B19" s="3" t="s">
-        <v>142</v>
+        <v>187</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -6847,7 +6965,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="2" t="s">
-        <v>143</v>
+        <v>188</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="1"/>
@@ -6884,7 +7002,7 @@
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="1" t="s">
-        <v>144</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>